<commit_message>
added required field indicator to imports
</commit_message>
<xml_diff>
--- a/Nada.UI/TestDistricts.xlsx
+++ b/Nada.UI/TestDistricts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jennifer\Documents\RTI\DB\TOT\021214 Geneva\files for training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\GitHub\NadaNTD\NadaNtd\Nada.UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>Alternate spelling names</t>
   </si>
   <si>
@@ -171,6 +165,12 @@
   </si>
   <si>
     <t>Zemelya</t>
+  </si>
+  <si>
+    <t>* Province</t>
+  </si>
+  <si>
+    <t>* District</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,69 +532,69 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>2013</v>
@@ -632,10 +632,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>2013</v>
@@ -673,10 +673,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D4">
         <v>2013</v>
@@ -714,10 +714,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>2013</v>
@@ -755,10 +755,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -796,10 +796,10 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>2013</v>
@@ -837,10 +837,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>2013</v>
@@ -878,10 +878,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D9">
         <v>2013</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>2013</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>2013</v>
@@ -1001,10 +1001,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>2013</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D13">
         <v>2013</v>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14">
         <v>2013</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15">
         <v>2013</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16">
         <v>2013</v>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>2013</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>2013</v>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>2013</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D20">
         <v>2013</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>2013</v>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22">
         <v>2013</v>
@@ -1452,10 +1452,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>2013</v>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24">
         <v>2013</v>
@@ -1534,10 +1534,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25">
         <v>2013</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>2013</v>

</xml_diff>